<commit_message>
sprint 4 done with some testing errors
</commit_message>
<xml_diff>
--- a/team5/Team05.xlsx
+++ b/team5/Team05.xlsx
@@ -10,14 +10,18 @@
     <sheet name="BACKLOG" sheetId="3" r:id="rId6"/>
     <sheet name="SPRINT 1" sheetId="4" r:id="rId7"/>
     <sheet name="SPRINT 2" sheetId="5" r:id="rId8"/>
-    <sheet name="User stories " sheetId="6" r:id="rId9"/>
-    <sheet name="Burdown Chart" sheetId="7" r:id="rId10"/>
+    <sheet name="SPRINT 3" sheetId="6" r:id="rId9"/>
+    <sheet name="SPRINT 4" sheetId="7" r:id="rId10"/>
+    <sheet name="User stories " sheetId="8" r:id="rId11"/>
+    <sheet name="Sprint -1 Burdown Chart" sheetId="9" r:id="rId12"/>
+    <sheet name="Sprint -2 BurnDown Chart" sheetId="10" r:id="rId13"/>
+    <sheet name="Sprint-3 BurnDown Chart" sheetId="11" r:id="rId14"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="336">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -847,6 +851,204 @@
     <t>Validate to see whether date of birth of parents and children are not spaced apart</t>
   </si>
   <si>
+    <t>Helping the team when a person from the team is looking for help</t>
+  </si>
+  <si>
+    <t>Delays in testing of the user stories</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>Act. Size</t>
+  </si>
+  <si>
+    <t>Act. Time</t>
+  </si>
+  <si>
+    <t>All Male members last names</t>
+  </si>
+  <si>
+    <t>T13.01</t>
+  </si>
+  <si>
+    <t>Check the name of the family</t>
+  </si>
+  <si>
+    <t>T13.02</t>
+  </si>
+  <si>
+    <t>Check the gender of the person</t>
+  </si>
+  <si>
+    <t>T13.03</t>
+  </si>
+  <si>
+    <t>Store the name of parent and sibling</t>
+  </si>
+  <si>
+    <t>T13.04</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether the last name</t>
+  </si>
+  <si>
+    <t>T18.01</t>
+  </si>
+  <si>
+    <t>Check the martial status of the person</t>
+  </si>
+  <si>
+    <t>T18.02</t>
+  </si>
+  <si>
+    <t>Check the martial status of the sibling</t>
+  </si>
+  <si>
+    <t>T18.03</t>
+  </si>
+  <si>
+    <t>Store the matial details details of the siblings</t>
+  </si>
+  <si>
+    <t>T18.04</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether the siblings are partners to each other</t>
+  </si>
+  <si>
+    <t>Check and store birth details</t>
+  </si>
+  <si>
+    <t>Check and store birth details of the sibling</t>
+  </si>
+  <si>
+    <t>Compare both to see whether siblings are born 8 months apart</t>
+  </si>
+  <si>
+    <t>T14.01</t>
+  </si>
+  <si>
+    <t>T14.02</t>
+  </si>
+  <si>
+    <t>T14.03</t>
+  </si>
+  <si>
+    <t>Check to see whether more than one sibling is born on the same date</t>
+  </si>
+  <si>
+    <t>T14.04</t>
+  </si>
+  <si>
+    <t>Validate to see that less than 5 siblings are born on a same date</t>
+  </si>
+  <si>
+    <t>T17.01</t>
+  </si>
+  <si>
+    <t>T17.02</t>
+  </si>
+  <si>
+    <t>Check the martial status of the parents</t>
+  </si>
+  <si>
+    <t>T17.03</t>
+  </si>
+  <si>
+    <t>Store the marital status of the person and parents</t>
+  </si>
+  <si>
+    <t>T17.04</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether the parents and children are partners to each other</t>
+  </si>
+  <si>
+    <t>T19.01</t>
+  </si>
+  <si>
+    <t>T19.02</t>
+  </si>
+  <si>
+    <t>Check the martial status of the cousin</t>
+  </si>
+  <si>
+    <t>T19.03</t>
+  </si>
+  <si>
+    <t>Store the date of marriage of  the person and cousin</t>
+  </si>
+  <si>
+    <t>T19.04</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether cousins are partners to each other</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>T22.01</t>
+  </si>
+  <si>
+    <t>Store the ID of the person</t>
+  </si>
+  <si>
+    <t>T22.02</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether the ID is unique fro all</t>
+  </si>
+  <si>
+    <t>T29.01</t>
+  </si>
+  <si>
+    <t>T29.02</t>
+  </si>
+  <si>
+    <t>Add to the list if the person is deceased</t>
+  </si>
+  <si>
+    <t>T29.03</t>
+  </si>
+  <si>
+    <t>Display the list</t>
+  </si>
+  <si>
+    <t>T23.01</t>
+  </si>
+  <si>
+    <t>Store the name of the person</t>
+  </si>
+  <si>
+    <t>T23.02</t>
+  </si>
+  <si>
+    <t>Store the birth date of the person</t>
+  </si>
+  <si>
+    <t>T23.03</t>
+  </si>
+  <si>
+    <t>Perform validation to see whether the name and birth date are unique</t>
+  </si>
+  <si>
+    <t>T31.01</t>
+  </si>
+  <si>
+    <t>T31.02</t>
+  </si>
+  <si>
+    <t>T31.03</t>
+  </si>
+  <si>
+    <t>Add to the list if the person is alive and single</t>
+  </si>
+  <si>
+    <t>Sprint -1 Burdown Chart</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -869,6 +1071,12 @@
   </si>
   <si>
     <t>Day-9</t>
+  </si>
+  <si>
+    <t>Sprint -2 BurnDown Chart</t>
+  </si>
+  <si>
+    <t>Sprint-3 BurnDown Chart</t>
   </si>
 </sst>
 </file>
@@ -879,7 +1087,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m/d"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -958,6 +1166,23 @@
       <color indexed="20"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="22"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
+      <color indexed="22"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="16"/>
+      <color indexed="25"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -997,7 +1222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1126,6 +1351,45 @@
       <left style="thin">
         <color indexed="13"/>
       </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="13"/>
       </right>
@@ -1285,7 +1549,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1439,25 +1703,73 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1467,6 +1779,21 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1501,6 +1828,11 @@
       <rgbColor rgb="ffd9d9d9"/>
       <rgbColor rgb="ff404040"/>
       <rgbColor rgb="ff595959"/>
+      <rgbColor rgb="fff1f1f1"/>
+      <rgbColor rgb="ffa7a7a7"/>
+      <rgbColor rgb="82d8d8d8"/>
+      <rgbColor rgb="89d8d8d8"/>
+      <rgbColor rgb="ff7f7f7f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1541,10 +1873,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.268234"/>
+          <c:x val="0.267966"/>
           <c:y val="0"/>
-          <c:w val="0.463531"/>
-          <c:h val="0.144395"/>
+          <c:w val="0.464068"/>
+          <c:h val="0.14699"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1560,10 +1892,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.067615"/>
-          <c:y val="0.144395"/>
-          <c:w val="0.927385"/>
-          <c:h val="0.665881"/>
+          <c:x val="0.0676933"/>
+          <c:y val="0.14699"/>
+          <c:w val="0.927307"/>
+          <c:h val="0.660892"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1590,7 +1922,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1693,7 +2025,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -1883,10 +2215,906 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.202625"/>
-          <c:y val="0.928616"/>
-          <c:w val="0.638608"/>
-          <c:h val="0.0713844"/>
+          <c:x val="0.18861"/>
+          <c:y val="0.927557"/>
+          <c:w val="0.667847"/>
+          <c:h val="0.0724427"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Helvetica Neue"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" i="0" strike="noStrike" sz="1600" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="A7A7A7"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" i="0" strike="noStrike" sz="1600" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="A7A7A7"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:rPr>
+              <a:t> BurnDown Chart For Sprint - 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.164333"/>
+          <c:y val="0"/>
+          <c:w val="0.671334"/>
+          <c:h val="0.158093"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0675077"/>
+          <c:y val="0.158093"/>
+          <c:w val="0.927492"/>
+          <c:h val="0.654772"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planned Work</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="A7A7A7"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Day-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day-9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Work Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="31750" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="A7A7A7"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Day-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day-9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint-3 BurnDown Chart'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="2094734552"/>
+        <c:axId val="2094734553"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2094734552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="A7A7A7"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734553"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2094734553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="F2F2F2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="A7A7A7"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.5"/>
+        <c:minorUnit val="0.75"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.216514"/>
+          <c:y val="0.929475"/>
+          <c:w val="0.609173"/>
+          <c:h val="0.0705246"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+              <a:solidFill>
+                <a:srgbClr val="A7A7A7"/>
+              </a:solidFill>
+              <a:latin typeface="Helvetica Neue"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat">
+      <a:solidFill>
+        <a:srgbClr val="F2F2F2"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" i="0" strike="noStrike" sz="1600" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="808080"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" i="0" strike="noStrike" sz="1600" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="808080"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:rPr>
+              <a:t>BurnDown Chart for Sprint 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.191746"/>
+          <c:y val="0"/>
+          <c:w val="0.616508"/>
+          <c:h val="0.158093"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0675941"/>
+          <c:y val="0.158093"/>
+          <c:w val="0.927406"/>
+          <c:h val="0.654772"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Planned Work</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Day-1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Day-3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Day-5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Day-7</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Day-9</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>6.000000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>5.000000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>5.000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4.000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2.000000</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Work Remaining</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="22225" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>Day-1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Day-3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Day-5</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Day-7</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Day-9</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>6.000000</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>4.000000</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4.000000</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3.000000</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2.000000</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="2094734552"/>
+        <c:axId val="2094734553"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2094734552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9">
+                  <a:alpha val="54000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9">
+                  <a:alpha val="51000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734553"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2094734553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9">
+                  <a:alpha val="54000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.5"/>
+        <c:minorUnit val="0.75"/>
+      </c:valAx>
+      <c:spPr>
+        <a:blipFill rotWithShape="1">
+          <a:blip r:embed="rId1"/>
+          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
+        </a:blipFill>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.216791"/>
+          <c:y val="0.929475"/>
+          <c:w val="0.609953"/>
+          <c:h val="0.0705246"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1939,13 +3167,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>782974</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>85012</xdr:rowOff>
+      <xdr:rowOff>82811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>291358</xdr:colOff>
+      <xdr:colOff>286196</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>63766</xdr:rowOff>
+      <xdr:rowOff>35878</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1953,8 +3181,78 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="782974" y="2229407"/>
-        <a:ext cx="4461385" cy="2318095"/>
+        <a:off x="782974" y="2213236"/>
+        <a:ext cx="4456223" cy="2277168"/>
+      </xdr:xfrm>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>243224</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>17137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584199</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30242</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="243224" y="1576697"/>
+        <a:ext cx="4468476" cy="2352446"/>
+      </xdr:xfrm>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>789324</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63492</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>299084</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76597</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="789324" y="1817997"/>
+        <a:ext cx="4462761" cy="2352446"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3039,14 +4337,14 @@
     <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
+    <row r="1" ht="15.25" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
+    <row r="2" ht="15.25" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3062,21 +4360,21 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
+    <row r="4" ht="15.25" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
+    <row r="5" ht="15.25" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" ht="15.25" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3096,7 +4394,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3206,7 +4504,7 @@
     <row r="19" ht="13" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" t="s" s="3">
-        <v>14</v>
+        <v>262</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -3219,14 +4517,14 @@
         <v>5</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>14</v>
+        <v>262</v>
       </c>
       <c r="E20" s="12"/>
     </row>
     <row r="21" ht="13" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" t="s" s="3">
-        <v>16</v>
+        <v>305</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3239,9 +4537,73 @@
         <v>5</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>16</v>
+        <v>305</v>
       </c>
       <c r="E22" s="21"/>
+    </row>
+    <row r="23">
+      <c r="B23" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s" s="3">
+        <v>325</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s" s="5">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s" s="3">
+        <v>334</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s" s="5">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s" s="3">
+        <v>335</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="4"/>
+      <c r="C30" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s" s="5">
+        <v>335</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3256,19 +4618,504 @@
     <hyperlink ref="D16" location="'SPRINT 1'!R1C1" tooltip="" display="SPRINT 1"/>
     <hyperlink ref="D18" location="'SPRINT 2'!R1C1" tooltip="" display="SPRINT 2"/>
     <hyperlink ref="D20" location="'User stories '!R1C1" tooltip="" display="User stories "/>
-    <hyperlink ref="D22" location="'Burdown Chart'!R1C1" tooltip="" display="Burdown Chart"/>
     <hyperlink ref="D12" location="'TEAM DETAILS'!R1C1" tooltip="" display="TEAM DETAILS"/>
     <hyperlink ref="D14" location="'BACKLOG'!R1C1" tooltip="" display="BACKLOG"/>
     <hyperlink ref="D16" location="'SPRINT 1'!R1C1" tooltip="" display="SPRINT 1"/>
     <hyperlink ref="D18" location="'SPRINT 2'!R1C1" tooltip="" display="SPRINT 2"/>
-    <hyperlink ref="D20" location="'User stories '!R1C1" tooltip="" display="User stories "/>
-    <hyperlink ref="D22" location="'Burdown Chart'!R1C1" tooltip="" display="Burdown Chart"/>
+    <hyperlink ref="D20" location="'SPRINT 3'!R1C1" tooltip="" display="SPRINT 3"/>
+    <hyperlink ref="D22" location="'SPRINT 4'!R1C1" tooltip="" display="SPRINT 4"/>
+    <hyperlink ref="D24" location="'User stories '!R1C1" tooltip="" display="User stories "/>
+    <hyperlink ref="D26" location="'Sprint -1 Burdown Chart'!R1C1" tooltip="" display="Sprint -1 Burdown Chart"/>
+    <hyperlink ref="D28" location="'Sprint -2 BurnDown Chart'!R1C1" tooltip="" display="Sprint -2 BurnDown Chart"/>
+    <hyperlink ref="D30" location="'Sprint-3 BurnDown Chart'!R1C1" tooltip="" display="Sprint-3 BurnDown Chart"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="6" width="10.8516" style="81" customWidth="1"/>
+    <col min="7" max="16384" width="10.8516" style="81" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.35" customHeight="1">
+      <c r="A1" t="s" s="55">
+        <v>326</v>
+      </c>
+      <c r="B1" t="s" s="55">
+        <v>327</v>
+      </c>
+      <c r="C1" t="s" s="55">
+        <v>328</v>
+      </c>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+    </row>
+    <row r="2" ht="15.35" customHeight="1">
+      <c r="A2" t="s" s="55">
+        <v>329</v>
+      </c>
+      <c r="B2" s="59">
+        <v>6</v>
+      </c>
+      <c r="C2" s="59">
+        <v>6</v>
+      </c>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+    </row>
+    <row r="3" ht="15.35" customHeight="1">
+      <c r="A3" t="s" s="55">
+        <v>330</v>
+      </c>
+      <c r="B3" s="59">
+        <v>5</v>
+      </c>
+      <c r="C3" s="59">
+        <v>4</v>
+      </c>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" t="s" s="55">
+        <v>331</v>
+      </c>
+      <c r="B4" s="59">
+        <v>5</v>
+      </c>
+      <c r="C4" s="59">
+        <v>4</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" t="s" s="55">
+        <v>332</v>
+      </c>
+      <c r="B5" s="59">
+        <v>4</v>
+      </c>
+      <c r="C5" s="59">
+        <v>3</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" t="s" s="55">
+        <v>333</v>
+      </c>
+      <c r="B6" s="59">
+        <v>2</v>
+      </c>
+      <c r="C6" s="59">
+        <v>2</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1">
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+    </row>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+    </row>
+    <row r="14" ht="15.35" customHeight="1">
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+    </row>
+    <row r="15" ht="15.35" customHeight="1">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+    </row>
+    <row r="17" ht="15.35" customHeight="1">
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+    </row>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+    </row>
+    <row r="19" ht="15.35" customHeight="1">
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+    </row>
+    <row r="20" ht="15.35" customHeight="1">
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+    </row>
+    <row r="21" ht="15.35" customHeight="1">
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="7" width="10.8516" style="82" customWidth="1"/>
+    <col min="8" max="16384" width="10.8516" style="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.35" customHeight="1">
+      <c r="A1" t="s" s="55">
+        <v>326</v>
+      </c>
+      <c r="B1" t="s" s="55">
+        <v>327</v>
+      </c>
+      <c r="C1" t="s" s="55">
+        <v>328</v>
+      </c>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+    </row>
+    <row r="2" ht="15.35" customHeight="1">
+      <c r="A2" t="s" s="55">
+        <v>329</v>
+      </c>
+      <c r="B2" s="59">
+        <v>6</v>
+      </c>
+      <c r="C2" s="59">
+        <v>6</v>
+      </c>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+    </row>
+    <row r="3" ht="15.35" customHeight="1">
+      <c r="A3" t="s" s="55">
+        <v>330</v>
+      </c>
+      <c r="B3" s="59">
+        <v>5</v>
+      </c>
+      <c r="C3" s="59">
+        <v>4</v>
+      </c>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" t="s" s="55">
+        <v>331</v>
+      </c>
+      <c r="B4" s="59">
+        <v>5</v>
+      </c>
+      <c r="C4" s="59">
+        <v>4</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" t="s" s="55">
+        <v>332</v>
+      </c>
+      <c r="B5" s="59">
+        <v>4</v>
+      </c>
+      <c r="C5" s="59">
+        <v>3</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" t="s" s="55">
+        <v>333</v>
+      </c>
+      <c r="B6" s="59">
+        <v>2</v>
+      </c>
+      <c r="C6" s="59">
+        <v>2</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1">
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+    </row>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" ht="15.35" customHeight="1">
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" ht="15.35" customHeight="1">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+    </row>
+    <row r="17" ht="15.35" customHeight="1">
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+    </row>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+    </row>
+    <row r="19" ht="15.35" customHeight="1">
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+    </row>
+    <row r="20" ht="15.35" customHeight="1">
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+    </row>
+    <row r="21" ht="15.35" customHeight="1">
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+    </row>
+    <row r="22" ht="15.35" customHeight="1">
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11706,7 +13553,7 @@
       </c>
       <c r="K44" s="39"/>
     </row>
-    <row r="45" ht="15.35" customHeight="1">
+    <row r="45" ht="15.25" customHeight="1">
       <c r="A45" s="7"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -11734,7 +13581,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" ht="15.35" customHeight="1">
+    <row r="47" ht="15.25" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -11792,7 +13639,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="12"/>
     </row>
-    <row r="51" ht="15.35" customHeight="1">
+    <row r="51" ht="15.25" customHeight="1">
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -11861,7 +13708,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -11916,17 +13763,27 @@
       <c r="C2" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E2" s="40">
         <v>20</v>
       </c>
       <c r="F2" s="40">
         <v>65</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="G2" s="40">
+        <v>15</v>
+      </c>
+      <c r="H2" s="40">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J2" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="3" ht="15.25" customHeight="1">
       <c r="A3" s="28"/>
@@ -11950,13 +13807,19 @@
       <c r="C4" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="I4" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J4" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="5" ht="15.25" customHeight="1">
       <c r="A5" t="s" s="33">
@@ -11968,13 +13831,19 @@
       <c r="C5" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="I5" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J5" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="6" ht="15.25" customHeight="1">
       <c r="A6" t="s" s="33">
@@ -11986,13 +13855,19 @@
       <c r="C6" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="I6" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J6" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="7" ht="15.25" customHeight="1">
       <c r="A7" t="s" s="33">
@@ -12004,13 +13879,19 @@
       <c r="C7" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="I7" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J7" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" t="s" s="33">
@@ -12022,13 +13903,19 @@
       <c r="C8" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="I8" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J8" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="28"/>
@@ -12052,17 +13939,27 @@
       <c r="C10" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E10" s="40">
         <v>15</v>
       </c>
       <c r="F10" s="40">
         <v>90</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
+      <c r="G10" s="42">
+        <v>18</v>
+      </c>
+      <c r="H10" s="42">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J10" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="11" ht="15.25" customHeight="1">
       <c r="A11" s="43"/>
@@ -12086,13 +13983,19 @@
       <c r="C12" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="I12" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J12" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="13" ht="15.25" customHeight="1">
       <c r="A13" t="s" s="33">
@@ -12104,13 +14007,19 @@
       <c r="C13" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
+      <c r="I13" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J13" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="14" ht="15.25" customHeight="1">
       <c r="A14" t="s" s="33">
@@ -12122,13 +14031,19 @@
       <c r="C14" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="I14" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J14" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="15" ht="16" customHeight="1">
       <c r="A15" t="s" s="33">
@@ -12140,13 +14055,19 @@
       <c r="C15" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="I15" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J15" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" t="s" s="33">
@@ -12158,13 +14079,19 @@
       <c r="C16" t="s" s="33">
         <v>28</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" t="s" s="39">
+        <v>174</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
+      <c r="I16" t="s" s="39">
+        <v>176</v>
+      </c>
+      <c r="J16" t="s" s="39">
+        <v>176</v>
+      </c>
     </row>
     <row r="17" ht="15.25" customHeight="1">
       <c r="A17" s="28"/>
@@ -12242,7 +14169,7 @@
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
     </row>
-    <row r="22" ht="15.35" customHeight="1">
+    <row r="22" ht="15.25" customHeight="1">
       <c r="A22" t="s" s="33">
         <v>213</v>
       </c>
@@ -12724,6 +14651,154 @@
         <v>176</v>
       </c>
     </row>
+    <row r="46" ht="15.35" customHeight="1">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" ht="16" customHeight="1">
+      <c r="A47" s="10"/>
+      <c r="B47" t="s" s="44">
+        <v>219</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="12"/>
+    </row>
+    <row r="48" ht="16" customHeight="1">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="12"/>
+    </row>
+    <row r="49" ht="16" customHeight="1">
+      <c r="A49" s="10"/>
+      <c r="B49" t="s" s="45">
+        <v>220</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="12"/>
+    </row>
+    <row r="50" ht="16" customHeight="1">
+      <c r="A50" s="10"/>
+      <c r="B50" t="s" s="46">
+        <v>221</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" ht="16" customHeight="1">
+      <c r="A51" s="10"/>
+      <c r="B51" t="s" s="46">
+        <v>260</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="12"/>
+    </row>
+    <row r="52" ht="16" customHeight="1">
+      <c r="A52" s="10"/>
+      <c r="B52" t="s" s="46">
+        <v>222</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="12"/>
+    </row>
+    <row r="53" ht="16" customHeight="1">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" ht="16" customHeight="1">
+      <c r="A54" s="10"/>
+      <c r="B54" t="s" s="45">
+        <v>223</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" ht="16" customHeight="1">
+      <c r="A55" s="10"/>
+      <c r="B55" t="s" s="46">
+        <v>224</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" ht="16" customHeight="1">
+      <c r="A56" s="20"/>
+      <c r="B56" t="s" s="47">
+        <v>261</v>
+      </c>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -12735,6 +14810,1878 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.8516" style="50" customWidth="1"/>
+    <col min="2" max="2" width="80.1719" style="50" customWidth="1"/>
+    <col min="3" max="10" width="10.8516" style="50" customWidth="1"/>
+    <col min="11" max="16384" width="10.8516" style="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" t="s" s="51">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s" s="51">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s" s="51">
+        <v>169</v>
+      </c>
+      <c r="E1" t="s" s="52">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s" s="52">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s" s="52">
+        <v>263</v>
+      </c>
+      <c r="H1" t="s" s="52">
+        <v>264</v>
+      </c>
+      <c r="I1" t="s" s="52">
+        <v>174</v>
+      </c>
+      <c r="J1" t="s" s="52">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" t="s" s="53">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s" s="54">
+        <v>265</v>
+      </c>
+      <c r="C2" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E2" s="56">
+        <v>25</v>
+      </c>
+      <c r="F2" s="56">
+        <v>75</v>
+      </c>
+      <c r="G2" s="56">
+        <v>15</v>
+      </c>
+      <c r="H2" s="56">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J2" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="57"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" t="s" s="54">
+        <v>266</v>
+      </c>
+      <c r="B4" t="s" s="35">
+        <v>267</v>
+      </c>
+      <c r="C4" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J4" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" t="s" s="54">
+        <v>268</v>
+      </c>
+      <c r="B5" t="s" s="35">
+        <v>269</v>
+      </c>
+      <c r="C5" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J5" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" t="s" s="54">
+        <v>270</v>
+      </c>
+      <c r="B6" t="s" s="35">
+        <v>271</v>
+      </c>
+      <c r="C6" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J6" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" t="s" s="54">
+        <v>272</v>
+      </c>
+      <c r="B7" t="s" s="35">
+        <v>273</v>
+      </c>
+      <c r="C7" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J7" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="57"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" t="s" s="53">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s" s="54">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E9" s="56">
+        <v>15</v>
+      </c>
+      <c r="F9" s="56">
+        <v>90</v>
+      </c>
+      <c r="G9" s="59">
+        <v>18</v>
+      </c>
+      <c r="H9" s="59">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J9" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" s="60"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+    </row>
+    <row r="11" ht="16" customHeight="1">
+      <c r="A11" t="s" s="54">
+        <v>274</v>
+      </c>
+      <c r="B11" t="s" s="35">
+        <v>275</v>
+      </c>
+      <c r="C11" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J11" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1">
+      <c r="A12" t="s" s="54">
+        <v>276</v>
+      </c>
+      <c r="B12" t="s" s="35">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J12" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1">
+      <c r="A13" t="s" s="54">
+        <v>278</v>
+      </c>
+      <c r="B13" t="s" s="35">
+        <v>279</v>
+      </c>
+      <c r="C13" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J13" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1">
+      <c r="A14" t="s" s="54">
+        <v>280</v>
+      </c>
+      <c r="B14" t="s" s="35">
+        <v>281</v>
+      </c>
+      <c r="C14" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J14" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" ht="16" customHeight="1">
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" ht="16" customHeight="1">
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+    </row>
+    <row r="17" ht="16" customHeight="1">
+      <c r="A17" t="s" s="54">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s" s="54">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="59">
+        <v>15</v>
+      </c>
+      <c r="F17" s="59">
+        <v>120</v>
+      </c>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+    </row>
+    <row r="18" ht="16" customHeight="1">
+      <c r="A18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+    </row>
+    <row r="19" ht="16" customHeight="1">
+      <c r="A19" t="s" s="54">
+        <v>266</v>
+      </c>
+      <c r="B19" t="s" s="35">
+        <v>282</v>
+      </c>
+      <c r="C19" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+    </row>
+    <row r="20" ht="16" customHeight="1">
+      <c r="A20" t="s" s="54">
+        <v>268</v>
+      </c>
+      <c r="B20" t="s" s="35">
+        <v>283</v>
+      </c>
+      <c r="C20" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+    </row>
+    <row r="21" ht="16" customHeight="1">
+      <c r="A21" t="s" s="54">
+        <v>270</v>
+      </c>
+      <c r="B21" t="s" s="35">
+        <v>284</v>
+      </c>
+      <c r="C21" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="22" ht="16" customHeight="1">
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+    </row>
+    <row r="23" ht="16" customHeight="1">
+      <c r="A23" t="s" s="54">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s" s="54">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D23" s="57"/>
+      <c r="E23" s="59">
+        <v>22</v>
+      </c>
+      <c r="F23" s="59">
+        <v>80</v>
+      </c>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+    </row>
+    <row r="24" ht="16" customHeight="1">
+      <c r="A24" s="60"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+    </row>
+    <row r="25" ht="16" customHeight="1">
+      <c r="A25" t="s" s="54">
+        <v>285</v>
+      </c>
+      <c r="B25" t="s" s="35">
+        <v>282</v>
+      </c>
+      <c r="C25" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+    </row>
+    <row r="26" ht="16" customHeight="1">
+      <c r="A26" t="s" s="54">
+        <v>286</v>
+      </c>
+      <c r="B26" t="s" s="35">
+        <v>283</v>
+      </c>
+      <c r="C26" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+    </row>
+    <row r="27" ht="16" customHeight="1">
+      <c r="A27" t="s" s="54">
+        <v>287</v>
+      </c>
+      <c r="B27" t="s" s="35">
+        <v>288</v>
+      </c>
+      <c r="C27" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="57"/>
+    </row>
+    <row r="28" ht="16" customHeight="1">
+      <c r="A28" t="s" s="54">
+        <v>289</v>
+      </c>
+      <c r="B28" t="s" s="35">
+        <v>290</v>
+      </c>
+      <c r="C28" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+    </row>
+    <row r="29" ht="16" customHeight="1">
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+    </row>
+    <row r="30" ht="16" customHeight="1">
+      <c r="A30" t="s" s="53">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s" s="54">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E30" s="59">
+        <v>20</v>
+      </c>
+      <c r="F30" s="59">
+        <v>120</v>
+      </c>
+      <c r="G30" s="59">
+        <v>15</v>
+      </c>
+      <c r="H30" s="59">
+        <v>80</v>
+      </c>
+      <c r="I30" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J30" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" ht="16" customHeight="1">
+      <c r="A31" s="60"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+    </row>
+    <row r="32" ht="16" customHeight="1">
+      <c r="A32" t="s" s="54">
+        <v>291</v>
+      </c>
+      <c r="B32" t="s" s="35">
+        <v>275</v>
+      </c>
+      <c r="C32" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J32" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" ht="16" customHeight="1">
+      <c r="A33" t="s" s="54">
+        <v>292</v>
+      </c>
+      <c r="B33" t="s" s="35">
+        <v>293</v>
+      </c>
+      <c r="C33" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J33" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" ht="16" customHeight="1">
+      <c r="A34" t="s" s="54">
+        <v>294</v>
+      </c>
+      <c r="B34" t="s" s="35">
+        <v>295</v>
+      </c>
+      <c r="C34" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J34" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" ht="16" customHeight="1">
+      <c r="A35" t="s" s="54">
+        <v>296</v>
+      </c>
+      <c r="B35" t="s" s="35">
+        <v>297</v>
+      </c>
+      <c r="C35" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J35" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" ht="16" customHeight="1">
+      <c r="A36" s="54"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+    </row>
+    <row r="37" ht="16" customHeight="1">
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+    </row>
+    <row r="38" ht="16" customHeight="1">
+      <c r="A38" t="s" s="53">
+        <v>96</v>
+      </c>
+      <c r="B38" t="s" s="54">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D38" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E38" s="59">
+        <v>18</v>
+      </c>
+      <c r="F38" s="59">
+        <v>110</v>
+      </c>
+      <c r="G38" s="59">
+        <v>24</v>
+      </c>
+      <c r="H38" s="59">
+        <v>100</v>
+      </c>
+      <c r="I38" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J38" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" ht="16" customHeight="1">
+      <c r="A39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+    </row>
+    <row r="40" ht="16" customHeight="1">
+      <c r="A40" t="s" s="54">
+        <v>298</v>
+      </c>
+      <c r="B40" t="s" s="35">
+        <v>275</v>
+      </c>
+      <c r="C40" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J40" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" ht="16" customHeight="1">
+      <c r="A41" t="s" s="54">
+        <v>299</v>
+      </c>
+      <c r="B41" t="s" s="35">
+        <v>300</v>
+      </c>
+      <c r="C41" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J41" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" ht="16" customHeight="1">
+      <c r="A42" t="s" s="54">
+        <v>301</v>
+      </c>
+      <c r="B42" t="s" s="35">
+        <v>302</v>
+      </c>
+      <c r="C42" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J42" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" ht="16" customHeight="1">
+      <c r="A43" t="s" s="54">
+        <v>303</v>
+      </c>
+      <c r="B43" t="s" s="35">
+        <v>304</v>
+      </c>
+      <c r="C43" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D43" t="s" s="55">
+        <v>174</v>
+      </c>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J43" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" ht="15.35" customHeight="1">
+      <c r="A44" s="57"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+    </row>
+    <row r="45" ht="15.35" customHeight="1">
+      <c r="A45" s="57"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+    </row>
+    <row r="46" ht="16" customHeight="1">
+      <c r="A46" s="62"/>
+      <c r="B46" t="s" s="44">
+        <v>219</v>
+      </c>
+      <c r="C46" s="63"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+    </row>
+    <row r="47" ht="16" customHeight="1">
+      <c r="A47" s="62"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+    </row>
+    <row r="48" ht="16" customHeight="1">
+      <c r="A48" s="62"/>
+      <c r="B48" t="s" s="65">
+        <v>220</v>
+      </c>
+      <c r="C48" s="63"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+    </row>
+    <row r="49" ht="16" customHeight="1">
+      <c r="A49" s="62"/>
+      <c r="B49" t="s" s="66">
+        <v>221</v>
+      </c>
+      <c r="C49" s="63"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+    </row>
+    <row r="50" ht="16" customHeight="1">
+      <c r="A50" s="62"/>
+      <c r="B50" t="s" s="66">
+        <v>222</v>
+      </c>
+      <c r="C50" s="63"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+    </row>
+    <row r="51" ht="16" customHeight="1">
+      <c r="A51" s="62"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+    </row>
+    <row r="52" ht="16" customHeight="1">
+      <c r="A52" s="62"/>
+      <c r="B52" t="s" s="65">
+        <v>223</v>
+      </c>
+      <c r="C52" s="63"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+    </row>
+    <row r="53" ht="16" customHeight="1">
+      <c r="A53" s="62"/>
+      <c r="B53" t="s" s="66">
+        <v>224</v>
+      </c>
+      <c r="C53" s="63"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+    </row>
+    <row r="54" ht="16" customHeight="1">
+      <c r="A54" s="62"/>
+      <c r="B54" t="s" s="67">
+        <v>225</v>
+      </c>
+      <c r="C54" s="63"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="10.8516" style="68" customWidth="1"/>
+    <col min="2" max="2" width="80.1719" style="68" customWidth="1"/>
+    <col min="3" max="10" width="10.8516" style="68" customWidth="1"/>
+    <col min="11" max="16384" width="10.8516" style="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16" customHeight="1">
+      <c r="A1" t="s" s="51">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s" s="51">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s" s="51">
+        <v>169</v>
+      </c>
+      <c r="E1" t="s" s="52">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s" s="52">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s" s="52">
+        <v>263</v>
+      </c>
+      <c r="H1" t="s" s="52">
+        <v>264</v>
+      </c>
+      <c r="I1" t="s" s="52">
+        <v>174</v>
+      </c>
+      <c r="J1" t="s" s="52">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" t="s" s="53">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s" s="54">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D2" s="55"/>
+      <c r="E2" s="56">
+        <v>25</v>
+      </c>
+      <c r="F2" s="56">
+        <v>75</v>
+      </c>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="57"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" t="s" s="54">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s" s="35">
+        <v>307</v>
+      </c>
+      <c r="C4" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" t="s" s="54">
+        <v>308</v>
+      </c>
+      <c r="B5" t="s" s="35">
+        <v>309</v>
+      </c>
+      <c r="C5" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D5" s="55"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" s="57"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" t="s" s="53">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s" s="54">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56">
+        <v>15</v>
+      </c>
+      <c r="F7" s="56">
+        <v>90</v>
+      </c>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" t="s" s="54">
+        <v>310</v>
+      </c>
+      <c r="B9" t="s" s="35">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" t="s" s="54">
+        <v>311</v>
+      </c>
+      <c r="B10" t="s" s="35">
+        <v>312</v>
+      </c>
+      <c r="C10" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+    </row>
+    <row r="11" ht="16" customHeight="1">
+      <c r="A11" t="s" s="54">
+        <v>313</v>
+      </c>
+      <c r="B11" t="s" s="35">
+        <v>314</v>
+      </c>
+      <c r="C11" t="s" s="54">
+        <v>28</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+    </row>
+    <row r="12" ht="16" customHeight="1">
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+    </row>
+    <row r="13" ht="16" customHeight="1">
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" ht="16" customHeight="1">
+      <c r="A14" t="s" s="54">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s" s="54">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D14" s="57"/>
+      <c r="E14" s="59">
+        <v>15</v>
+      </c>
+      <c r="F14" s="59">
+        <v>120</v>
+      </c>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+    </row>
+    <row r="15" ht="16" customHeight="1">
+      <c r="A15" s="60"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" ht="16" customHeight="1">
+      <c r="A16" t="s" s="54">
+        <v>266</v>
+      </c>
+      <c r="B16" t="s" s="35">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="57"/>
+    </row>
+    <row r="17" ht="16" customHeight="1">
+      <c r="A17" t="s" s="54">
+        <v>268</v>
+      </c>
+      <c r="B17" t="s" s="35">
+        <v>283</v>
+      </c>
+      <c r="C17" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+    </row>
+    <row r="18" ht="16" customHeight="1">
+      <c r="A18" t="s" s="54">
+        <v>270</v>
+      </c>
+      <c r="B18" t="s" s="35">
+        <v>284</v>
+      </c>
+      <c r="C18" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+    </row>
+    <row r="19" ht="16" customHeight="1">
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+    </row>
+    <row r="20" ht="16" customHeight="1">
+      <c r="A20" t="s" s="54">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s" s="54">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="59">
+        <v>22</v>
+      </c>
+      <c r="F20" s="59">
+        <v>80</v>
+      </c>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+    </row>
+    <row r="21" ht="16" customHeight="1">
+      <c r="A21" s="60"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="22" ht="16" customHeight="1">
+      <c r="A22" t="s" s="54">
+        <v>285</v>
+      </c>
+      <c r="B22" t="s" s="35">
+        <v>282</v>
+      </c>
+      <c r="C22" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+    </row>
+    <row r="23" ht="16" customHeight="1">
+      <c r="A23" t="s" s="54">
+        <v>286</v>
+      </c>
+      <c r="B23" t="s" s="35">
+        <v>283</v>
+      </c>
+      <c r="C23" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+    </row>
+    <row r="24" ht="16" customHeight="1">
+      <c r="A24" t="s" s="54">
+        <v>287</v>
+      </c>
+      <c r="B24" t="s" s="35">
+        <v>288</v>
+      </c>
+      <c r="C24" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+    </row>
+    <row r="25" ht="16" customHeight="1">
+      <c r="A25" t="s" s="54">
+        <v>289</v>
+      </c>
+      <c r="B25" t="s" s="35">
+        <v>290</v>
+      </c>
+      <c r="C25" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+    </row>
+    <row r="26" ht="16" customHeight="1">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+    </row>
+    <row r="27" ht="16" customHeight="1">
+      <c r="A27" t="s" s="53">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s" s="54">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D27" s="55"/>
+      <c r="E27" s="59">
+        <v>20</v>
+      </c>
+      <c r="F27" s="59">
+        <v>120</v>
+      </c>
+      <c r="G27" s="59">
+        <v>18</v>
+      </c>
+      <c r="H27" s="59">
+        <v>75</v>
+      </c>
+      <c r="I27" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J27" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" ht="16" customHeight="1">
+      <c r="A28" s="60"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+    </row>
+    <row r="29" ht="16" customHeight="1">
+      <c r="A29" t="s" s="54">
+        <v>315</v>
+      </c>
+      <c r="B29" t="s" s="35">
+        <v>316</v>
+      </c>
+      <c r="C29" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D29" s="55"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+    </row>
+    <row r="30" ht="16" customHeight="1">
+      <c r="A30" t="s" s="54">
+        <v>317</v>
+      </c>
+      <c r="B30" t="s" s="35">
+        <v>318</v>
+      </c>
+      <c r="C30" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D30" s="55"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+    </row>
+    <row r="31" ht="16" customHeight="1">
+      <c r="A31" t="s" s="54">
+        <v>319</v>
+      </c>
+      <c r="B31" t="s" s="35">
+        <v>320</v>
+      </c>
+      <c r="C31" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D31" s="55"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+    </row>
+    <row r="32" ht="16" customHeight="1">
+      <c r="A32" s="54"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+    </row>
+    <row r="33" ht="16" customHeight="1">
+      <c r="A33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+    </row>
+    <row r="34" ht="16" customHeight="1">
+      <c r="A34" t="s" s="53">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s" s="54">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D34" s="55"/>
+      <c r="E34" s="59">
+        <v>18</v>
+      </c>
+      <c r="F34" s="59">
+        <v>110</v>
+      </c>
+      <c r="G34" s="59">
+        <v>20</v>
+      </c>
+      <c r="H34" s="59">
+        <v>100</v>
+      </c>
+      <c r="I34" t="s" s="55">
+        <v>176</v>
+      </c>
+      <c r="J34" t="s" s="55">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" ht="16" customHeight="1">
+      <c r="A35" s="60"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+    </row>
+    <row r="36" ht="16" customHeight="1">
+      <c r="A36" t="s" s="54">
+        <v>321</v>
+      </c>
+      <c r="B36" t="s" s="35">
+        <v>275</v>
+      </c>
+      <c r="C36" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D36" s="55"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+    </row>
+    <row r="37" ht="16" customHeight="1">
+      <c r="A37" t="s" s="54">
+        <v>322</v>
+      </c>
+      <c r="B37" t="s" s="35">
+        <v>184</v>
+      </c>
+      <c r="C37" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D37" s="55"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+    </row>
+    <row r="38" ht="16" customHeight="1">
+      <c r="A38" t="s" s="54">
+        <v>323</v>
+      </c>
+      <c r="B38" t="s" s="35">
+        <v>324</v>
+      </c>
+      <c r="C38" t="s" s="54">
+        <v>23</v>
+      </c>
+      <c r="D38" s="55"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="55"/>
+    </row>
+    <row r="39" ht="16" customHeight="1">
+      <c r="A39" s="54"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+    </row>
+    <row r="40" ht="15.35" customHeight="1">
+      <c r="A40" s="57"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="57"/>
+    </row>
+    <row r="41" ht="15.35" customHeight="1">
+      <c r="A41" s="57"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+    </row>
+    <row r="42" ht="16" customHeight="1">
+      <c r="A42" s="62"/>
+      <c r="B42" t="s" s="44">
+        <v>219</v>
+      </c>
+      <c r="C42" s="63"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+    </row>
+    <row r="43" ht="16" customHeight="1">
+      <c r="A43" s="62"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+    </row>
+    <row r="44" ht="16" customHeight="1">
+      <c r="A44" s="62"/>
+      <c r="B44" t="s" s="65">
+        <v>220</v>
+      </c>
+      <c r="C44" s="63"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+    </row>
+    <row r="45" ht="16" customHeight="1">
+      <c r="A45" s="62"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+    </row>
+    <row r="46" ht="16" customHeight="1">
+      <c r="A46" s="62"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+    </row>
+    <row r="47" ht="16" customHeight="1">
+      <c r="A47" s="62"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+    </row>
+    <row r="48" ht="16" customHeight="1">
+      <c r="A48" s="62"/>
+      <c r="B48" t="s" s="65">
+        <v>223</v>
+      </c>
+      <c r="C48" s="63"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+    </row>
+    <row r="49" ht="16" customHeight="1">
+      <c r="A49" s="62"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+    </row>
+    <row r="50" ht="16" customHeight="1">
+      <c r="A50" s="62"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12744,88 +16691,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="16.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="50" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="50" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="69" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.5" customHeight="1">
-      <c r="A1" t="s" s="51">
+      <c r="A1" t="s" s="70">
         <v>5</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
     </row>
     <row r="4" ht="14.75" customHeight="1">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" ht="14.75" customHeight="1">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
     </row>
     <row r="6" ht="14.75" customHeight="1">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
     </row>
     <row r="7" ht="14.75" customHeight="1">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
     </row>
     <row r="8" ht="14.75" customHeight="1">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
     </row>
     <row r="9" ht="14.75" customHeight="1">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
     </row>
     <row r="10" ht="14.75" customHeight="1">
-      <c r="A10" s="58"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
     </row>
     <row r="11" ht="14.75" customHeight="1">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12839,7 +16786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G24"/>
   <sheetViews>
@@ -12847,28 +16794,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="10.8516" style="61" customWidth="1"/>
-    <col min="8" max="16384" width="10.8516" style="61" customWidth="1"/>
+    <col min="1" max="7" width="10.8516" style="80" customWidth="1"/>
+    <col min="8" max="16384" width="10.8516" style="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
+    <row r="1" ht="15.25" customHeight="1">
       <c r="A1" t="s" s="39">
-        <v>260</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s" s="39">
-        <v>261</v>
+        <v>327</v>
       </c>
       <c r="C1" t="s" s="39">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
+    <row r="2" ht="15.25" customHeight="1">
       <c r="A2" t="s" s="39">
-        <v>263</v>
+        <v>329</v>
       </c>
       <c r="B2" s="42">
         <v>6</v>
@@ -12881,9 +16828,9 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
+    <row r="3" ht="15.25" customHeight="1">
       <c r="A3" t="s" s="39">
-        <v>264</v>
+        <v>330</v>
       </c>
       <c r="B3" s="42">
         <v>4</v>
@@ -12896,9 +16843,9 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
+    <row r="4" ht="15.25" customHeight="1">
       <c r="A4" t="s" s="39">
-        <v>265</v>
+        <v>331</v>
       </c>
       <c r="B4" s="42">
         <v>4</v>
@@ -12911,9 +16858,9 @@
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
+    <row r="5" ht="15.25" customHeight="1">
       <c r="A5" t="s" s="39">
-        <v>266</v>
+        <v>332</v>
       </c>
       <c r="B5" s="42">
         <v>3</v>
@@ -12926,9 +16873,9 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
+    <row r="6" ht="15.25" customHeight="1">
       <c r="A6" t="s" s="39">
-        <v>267</v>
+        <v>333</v>
       </c>
       <c r="B6" s="42">
         <v>2</v>
@@ -12941,7 +16888,7 @@
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
+    <row r="7" ht="15.25" customHeight="1">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -12950,7 +16897,7 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
+    <row r="8" ht="15.25" customHeight="1">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -12959,7 +16906,7 @@
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
+    <row r="9" ht="15.25" customHeight="1">
       <c r="A9" s="28"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
@@ -12968,7 +16915,7 @@
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
+    <row r="10" ht="15.25" customHeight="1">
       <c r="A10" s="28"/>
       <c r="B10" s="28"/>
       <c r="C10" s="28"/>
@@ -12977,7 +16924,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" ht="15.35" customHeight="1">
+    <row r="11" ht="15.25" customHeight="1">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -12986,7 +16933,7 @@
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
     </row>
-    <row r="12" ht="15.35" customHeight="1">
+    <row r="12" ht="15.25" customHeight="1">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -12995,7 +16942,7 @@
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
     </row>
-    <row r="13" ht="15.35" customHeight="1">
+    <row r="13" ht="15.25" customHeight="1">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -13004,7 +16951,7 @@
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
     </row>
-    <row r="14" ht="15.35" customHeight="1">
+    <row r="14" ht="15.25" customHeight="1">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -13013,7 +16960,7 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
     </row>
-    <row r="15" ht="15.35" customHeight="1">
+    <row r="15" ht="15.25" customHeight="1">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -13022,7 +16969,7 @@
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" ht="15.35" customHeight="1">
+    <row r="16" ht="15.25" customHeight="1">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -13031,7 +16978,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" ht="15.35" customHeight="1">
+    <row r="17" ht="15.25" customHeight="1">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -13040,7 +16987,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" ht="15.35" customHeight="1">
+    <row r="18" ht="15.25" customHeight="1">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -13049,7 +16996,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" ht="15.35" customHeight="1">
+    <row r="19" ht="15.25" customHeight="1">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -13058,7 +17005,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" ht="15.35" customHeight="1">
+    <row r="20" ht="15.25" customHeight="1">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="28"/>
@@ -13067,7 +17014,7 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" ht="15.35" customHeight="1">
+    <row r="21" ht="15.25" customHeight="1">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
@@ -13076,7 +17023,7 @@
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" ht="15.35" customHeight="1">
+    <row r="22" ht="15.25" customHeight="1">
       <c r="A22" s="28"/>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -13085,7 +17032,7 @@
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" ht="15.35" customHeight="1">
+    <row r="23" ht="15.25" customHeight="1">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -13094,7 +17041,7 @@
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
     </row>
-    <row r="24" ht="15.35" customHeight="1">
+    <row r="24" ht="15.25" customHeight="1">
       <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>

</xml_diff>